<commit_message>
Working gud both dash and API Response
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/APIData.xlsx
+++ b/src/test/resources/testData/APIData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7200" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7200" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="apiGET" sheetId="1" r:id="rId1"/>
@@ -765,7 +765,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -843,7 +843,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>16</v>
@@ -1209,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1296,7 +1296,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>16</v>
@@ -1731,7 +1731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1823,7 +1823,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>16</v>
@@ -1871,7 +1871,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>16</v>
@@ -1919,7 +1919,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>16</v>
@@ -1967,7 +1967,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>16</v>
@@ -2015,7 +2015,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>16</v>
@@ -2063,7 +2063,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Initial commit - Excel to DB automation framework
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/APIData.xlsx
+++ b/src/test/resources/testData/APIData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="99">
   <si>
     <t>caseID</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>TC003</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>TC004</t>
@@ -229,9 +226,6 @@
   </si>
   <si>
     <t>{"bookId":1,"customerName1":"Jon"}</t>
-  </si>
-  <si>
-    <t>books/</t>
   </si>
   <si>
     <t>mail</t>
@@ -892,7 +886,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -922,10 +916,10 @@
         <v>14</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R1" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="42.75" x14ac:dyDescent="0.2">
@@ -933,13 +927,13 @@
         <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>18</v>
@@ -948,7 +942,7 @@
         <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>19</v>
@@ -959,10 +953,10 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -974,25 +968,25 @@
         <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>20</v>
@@ -1020,10 +1014,10 @@
         <v>23</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>18</v>
@@ -1035,16 +1029,16 @@
         <v>18</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>21</v>
@@ -1057,16 +1051,16 @@
     </row>
     <row r="5" spans="1:19" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>18</v>
@@ -1075,10 +1069,10 @@
         <v>18</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>20</v>
@@ -1090,10 +1084,10 @@
         <v>18</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -1328,7 +1322,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1374,7 +1370,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1389,7 +1385,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>10</v>
@@ -1407,10 +1403,10 @@
         <v>14</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S1" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1418,13 +1414,13 @@
         <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>18</v>
@@ -1433,28 +1429,28 @@
         <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="N2" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
@@ -1468,40 +1464,40 @@
         <v>23</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="N3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" s="11"/>
       <c r="P3" s="3"/>
@@ -1515,40 +1511,40 @@
         <v>23</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="N4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -1556,46 +1552,46 @@
     </row>
     <row r="5" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="I5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="M5" s="23" t="s">
+      <c r="N5" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
@@ -1603,20 +1599,20 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C13" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E14" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C15" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1636,7 +1632,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1670,7 +1668,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>4</v>
@@ -1679,7 +1677,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="20" t="s">
         <v>6</v>
@@ -1694,7 +1692,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M1" s="20" t="s">
         <v>10</v>
@@ -1712,10 +1710,10 @@
         <v>14</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S1" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="99.75" x14ac:dyDescent="0.2">
@@ -1723,13 +1721,13 @@
         <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>18</v>
@@ -1738,28 +1736,28 @@
         <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
@@ -1779,7 +1777,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1823,7 +1821,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="20" t="s">
         <v>6</v>
@@ -1853,10 +1851,10 @@
         <v>14</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R1" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="42.75" x14ac:dyDescent="0.2">
@@ -1864,10 +1862,10 @@
         <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>17</v>
@@ -1879,13 +1877,13 @@
         <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -1895,7 +1893,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1950,7 +1948,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1959,7 +1957,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1974,7 +1972,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>10</v>
@@ -1992,10 +1990,10 @@
         <v>14</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S1" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2009,7 +2007,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>18</v>
@@ -2018,13 +2016,13 @@
         <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>21</v>
@@ -2033,13 +2031,13 @@
         <v>18</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O2" s="10"/>
       <c r="P2" s="5"/>
@@ -2058,19 +2056,19 @@
         <v>16</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>20</v>
@@ -2079,16 +2077,16 @@
         <v>21</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N3" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
@@ -2107,37 +2105,37 @@
         <v>16</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="I4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
@@ -2156,19 +2154,19 @@
         <v>16</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>20</v>
@@ -2177,16 +2175,16 @@
         <v>21</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
@@ -2205,37 +2203,37 @@
         <v>16</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="I6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
@@ -2254,19 +2252,19 @@
         <v>16</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>20</v>
@@ -2275,16 +2273,16 @@
         <v>21</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
@@ -2303,7 +2301,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>18</v>
@@ -2312,13 +2310,13 @@
         <v>18</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>21</v>
@@ -2327,13 +2325,13 @@
         <v>18</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
@@ -2352,19 +2350,19 @@
         <v>16</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>20</v>
@@ -2373,16 +2371,16 @@
         <v>21</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N9" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
@@ -2401,7 +2399,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>18</v>
@@ -2410,13 +2408,13 @@
         <v>18</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>21</v>
@@ -2425,13 +2423,13 @@
         <v>18</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
@@ -2447,40 +2445,40 @@
         <v>23</v>
       </c>
       <c r="C11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
@@ -2499,19 +2497,19 @@
         <v>16</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>20</v>
@@ -2520,16 +2518,16 @@
         <v>21</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
@@ -2539,7 +2537,7 @@
     </row>
     <row r="13" spans="1:19" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>23</v>
@@ -2548,7 +2546,7 @@
         <v>16</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>18</v>
@@ -2557,13 +2555,13 @@
         <v>18</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>21</v>
@@ -2572,13 +2570,13 @@
         <v>18</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -2588,7 +2586,7 @@
     </row>
     <row r="14" spans="1:19" ht="57" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>23</v>
@@ -2606,10 +2604,10 @@
         <v>18</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>20</v>
@@ -2618,16 +2616,16 @@
         <v>21</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N14" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -2637,13 +2635,13 @@
     </row>
     <row r="15" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>17</v>
@@ -2655,28 +2653,28 @@
         <v>18</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
@@ -2686,7 +2684,7 @@
     </row>
     <row r="16" spans="1:19" ht="57" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>23</v>
@@ -2704,10 +2702,10 @@
         <v>18</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>20</v>
@@ -2716,16 +2714,16 @@
         <v>21</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -2735,7 +2733,7 @@
     </row>
     <row r="17" spans="1:19" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>23</v>
@@ -2744,7 +2742,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>18</v>
@@ -2753,13 +2751,13 @@
         <v>18</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>21</v>
@@ -2768,13 +2766,13 @@
         <v>18</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -2784,7 +2782,7 @@
     </row>
     <row r="18" spans="1:19" ht="57" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>23</v>
@@ -2802,10 +2800,10 @@
         <v>18</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>20</v>
@@ -2814,16 +2812,16 @@
         <v>21</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
@@ -2833,13 +2831,13 @@
     </row>
     <row r="19" spans="1:19" ht="57" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>17</v>
@@ -2851,28 +2849,28 @@
         <v>18</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N19" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
@@ -2882,7 +2880,7 @@
     </row>
     <row r="20" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>23</v>
@@ -2891,7 +2889,7 @@
         <v>16</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>18</v>
@@ -2900,13 +2898,13 @@
         <v>18</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>21</v>
@@ -2915,13 +2913,13 @@
         <v>18</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M20" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
@@ -2931,13 +2929,13 @@
     </row>
     <row r="21" spans="1:19" ht="57" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>17</v>
@@ -2949,28 +2947,28 @@
         <v>18</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N21" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
@@ -2980,7 +2978,7 @@
     </row>
     <row r="22" spans="1:19" ht="57" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>23</v>
@@ -2998,10 +2996,10 @@
         <v>18</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>20</v>
@@ -3010,16 +3008,16 @@
         <v>21</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N22" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
@@ -3029,7 +3027,7 @@
     </row>
     <row r="23" spans="1:19" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>23</v>
@@ -3038,7 +3036,7 @@
         <v>16</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>18</v>
@@ -3047,13 +3045,13 @@
         <v>18</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>21</v>
@@ -3062,13 +3060,13 @@
         <v>18</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -3078,7 +3076,7 @@
     </row>
     <row r="24" spans="1:19" ht="57" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>23</v>
@@ -3096,10 +3094,10 @@
         <v>18</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>20</v>
@@ -3108,16 +3106,16 @@
         <v>21</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
@@ -3127,13 +3125,13 @@
     </row>
     <row r="25" spans="1:19" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>17</v>
@@ -3145,28 +3143,28 @@
         <v>18</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N25" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
@@ -3176,7 +3174,7 @@
     </row>
     <row r="26" spans="1:19" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>23</v>
@@ -3194,10 +3192,10 @@
         <v>18</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>20</v>
@@ -3206,16 +3204,16 @@
         <v>21</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N26" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
@@ -3225,16 +3223,16 @@
     </row>
     <row r="27" spans="1:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>18</v>
@@ -3243,13 +3241,13 @@
         <v>18</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>18</v>
@@ -3258,7 +3256,7 @@
         <v>18</v>
       </c>
       <c r="L27" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M27" s="31"/>
       <c r="N27" s="32"/>
@@ -3270,16 +3268,16 @@
     </row>
     <row r="28" spans="1:19" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>18</v>
@@ -3288,10 +3286,10 @@
         <v>18</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>20</v>
@@ -3315,16 +3313,16 @@
     </row>
     <row r="29" spans="1:19" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>18</v>
@@ -3333,10 +3331,10 @@
         <v>18</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>20</v>
@@ -3360,16 +3358,16 @@
     </row>
     <row r="30" spans="1:19" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>97</v>
-      </c>
       <c r="D30" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>18</v>
@@ -3378,10 +3376,10 @@
         <v>18</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>20</v>
@@ -3405,17 +3403,17 @@
     </row>
     <row r="31" spans="1:19" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>100</v>
-      </c>
       <c r="E31" s="11" t="s">
         <v>18</v>
       </c>
@@ -3423,10 +3421,10 @@
         <v>18</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H31" s="33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>20</v>

</xml_diff>